<commit_message>
Update Group5 Estimated Effort Iteration 5 Begin.xlsx
</commit_message>
<xml_diff>
--- a/Group5 Estimated Effort Iteration 5 Begin.xlsx
+++ b/Group5 Estimated Effort Iteration 5 Begin.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Donald\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE8E0E2A-BA39-414C-B01F-436C37B2F60E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0A0DD36-2186-4B83-A41B-5DC44EA2472C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1758,8 +1758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:AE97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B79" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="B73" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G93" sqref="G93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
@@ -4572,8 +4572,8 @@
       <c r="E92" s="98"/>
       <c r="F92" s="99"/>
       <c r="G92" s="100">
-        <f>SUM(F93:F93)</f>
-        <v>2</v>
+        <f>SUM(F93:F94)</f>
+        <v>4</v>
       </c>
       <c r="H92" s="68"/>
       <c r="I92" s="72"/>

</xml_diff>